<commit_message>
Update API base URL and improve data processing
</commit_message>
<xml_diff>
--- a/FicherosEntrada/2024/Exportaciones-CEUTA-02-07/Oferta-FP-24-25_CEUTA_VACANTES_02-07.xlsx
+++ b/FicherosEntrada/2024/Exportaciones-CEUTA-02-07/Oferta-FP-24-25_CEUTA_VACANTES_02-07.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GBNEE" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="192">
   <si>
     <t xml:space="preserve">codigo centro </t>
   </si>
@@ -659,6 +659,12 @@
     <t xml:space="preserve">Desarrollo de videojuegos y Realidad Virtual (VESPERTINO)</t>
   </si>
   <si>
+    <t xml:space="preserve">Especialización en Ciberseguridad en Entornos de las Tecnologías de la Información  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mantenimiento de Vehículos Híbridos y Eléctricos</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -712,7 +718,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -779,8 +785,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,6 +823,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -888,7 +908,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -910,6 +930,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -949,6 +973,30 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -959,6 +1007,14 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1044,7 +1100,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1811,8 +1867,8 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2304,14 +2360,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>51000286</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="C25" s="6" t="n">
         <v>121110021</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -2900,10 +2956,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J61" activeCellId="0" sqref="J61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2912,7 +2968,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="50.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="43.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.4"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.99"/>
@@ -2933,26 +2989,26 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -2965,24 +3021,26 @@
       <c r="D2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="10" t="n">
+      <c r="E2" s="11" t="n">
         <v>10437</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="12" t="n">
         <v>190</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="11" t="n">
+        <v>10437</v>
+      </c>
+      <c r="J2" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -2995,24 +3053,26 @@
       <c r="D3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="10" t="n">
+      <c r="E3" s="11" t="n">
         <v>10438</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="11" t="n">
+      <c r="G3" s="12" t="n">
         <v>130</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="11" t="n">
+        <v>10438</v>
+      </c>
+      <c r="J3" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3025,24 +3085,26 @@
       <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="11" t="n">
         <v>10439</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="11" t="n">
+      <c r="G4" s="12" t="n">
         <v>100</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I4" s="11" t="n">
+        <v>10439</v>
+      </c>
+      <c r="J4" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3055,24 +3117,26 @@
       <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="E5" s="11" t="n">
         <v>10440</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="11" t="n">
+      <c r="G5" s="12" t="n">
         <v>250</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="11" t="n">
+        <v>10440</v>
+      </c>
+      <c r="J5" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3085,24 +3149,26 @@
       <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="10" t="n">
+      <c r="E6" s="11" t="n">
         <v>10441</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="11" t="n">
+      <c r="G6" s="12" t="n">
         <v>100</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="11" t="n">
+        <v>10441</v>
+      </c>
+      <c r="J6" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3115,54 +3181,58 @@
       <c r="D7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="10" t="n">
+      <c r="E7" s="14" t="n">
         <v>10156</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="11" t="n">
+      <c r="G7" s="12" t="n">
         <v>70</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="I7" s="14" t="n">
+        <v>10156</v>
+      </c>
+      <c r="J7" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="n">
         <v>51004772</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="15" t="n">
         <v>121121013</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="10" t="n">
-        <v>11709</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="H8" s="5" t="n">
+      <c r="E8" s="17" t="n">
+        <v>156</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="19" t="n">
+        <v>70</v>
+      </c>
+      <c r="H8" s="20" t="n">
         <v>60</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="17" t="n">
+        <v>156</v>
+      </c>
+      <c r="J8" s="18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3175,24 +3245,26 @@
       <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="10" t="n">
-        <v>11708</v>
+      <c r="E9" s="11" t="n">
+        <v>11709</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="11" t="n">
-        <v>35</v>
+        <v>71</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>100</v>
       </c>
       <c r="H9" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="11" t="n">
+        <v>11709</v>
+      </c>
+      <c r="J9" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3205,23 +3277,26 @@
       <c r="D10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="13" t="n">
-        <v>10446</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="11" t="n">
+        <v>11708</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="12" t="n">
+        <v>35</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>11708</v>
+      </c>
+      <c r="J10" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3234,11 +3309,11 @@
       <c r="D11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="13" t="n">
-        <v>10448</v>
+      <c r="E11" s="14" t="n">
+        <v>10446</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="1" t="n">
         <v>170</v>
@@ -3246,11 +3321,14 @@
       <c r="H11" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I11" s="14" t="n">
+        <v>10446</v>
+      </c>
       <c r="J11" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3263,23 +3341,26 @@
       <c r="D12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="13" t="n">
-        <v>10442</v>
+      <c r="E12" s="14" t="n">
+        <v>10448</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I12" s="14" t="n">
+        <v>10448</v>
+      </c>
       <c r="J12" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3292,11 +3373,11 @@
       <c r="D13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="13" t="n">
-        <v>10443</v>
+      <c r="E13" s="14" t="n">
+        <v>10442</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>150</v>
@@ -3304,11 +3385,14 @@
       <c r="H13" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I13" s="14" t="n">
+        <v>10442</v>
+      </c>
       <c r="J13" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>51004772</v>
       </c>
@@ -3321,170 +3405,186 @@
       <c r="D14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="13" t="n">
-        <v>10451</v>
+      <c r="E14" s="14" t="n">
+        <v>442</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I14" s="14" t="n">
+        <v>10442</v>
+      </c>
       <c r="J14" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
+        <v>51004772</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>121121013</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="14" t="n">
+        <v>10443</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I15" s="14" t="n">
+        <v>10443</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>51004772</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>121121013</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="14" t="n">
+        <v>10451</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I16" s="14" t="n">
+        <v>10451</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="n">
         <v>51000286</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C17" s="15" t="n">
         <v>121110023</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D17" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="6" t="n">
-        <v>10367</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E17" s="17" t="n">
+        <v>367</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G17" s="15" t="n">
         <v>60</v>
       </c>
-      <c r="H15" s="1" t="n">
+      <c r="H17" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J15" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="I17" s="17" t="n">
+        <v>367</v>
+      </c>
+      <c r="J17" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="n">
         <v>51000286</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C18" s="15" t="n">
         <v>121110023</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="6" t="n">
-        <v>10238</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E18" s="17" t="n">
+        <v>238</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G18" s="15" t="n">
         <v>130</v>
       </c>
-      <c r="H16" s="1" t="n">
+      <c r="H18" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J16" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="I18" s="17" t="n">
+        <v>238</v>
+      </c>
+      <c r="J18" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="n">
         <v>51000286</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C19" s="15" t="n">
         <v>121110023</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="6" t="n">
-        <v>10365</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E19" s="17" t="n">
+        <v>365</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="G19" s="15" t="n">
         <v>140</v>
       </c>
-      <c r="H17" s="1" t="n">
+      <c r="H19" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J17" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>51000304</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>121124013</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="13" t="n">
-        <v>10046</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="4" t="n">
-        <v>290</v>
-      </c>
-      <c r="H18" s="4" t="n">
-        <v>60</v>
-      </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>51000304</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>121124013</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="13" t="n">
-        <v>10047</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="4" t="n">
-        <v>290</v>
-      </c>
-      <c r="H19" s="4" t="n">
-        <v>60</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="17" t="n">
+        <v>365</v>
+      </c>
+      <c r="J19" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3497,24 +3597,26 @@
       <c r="D20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="13" t="n">
-        <v>10026</v>
+      <c r="E20" s="14" t="n">
+        <v>10046</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>190</v>
+        <v>290</v>
       </c>
       <c r="H20" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="14" t="n">
+        <v>10046</v>
+      </c>
       <c r="J20" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3527,84 +3629,90 @@
       <c r="D21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="13" t="n">
-        <v>11709</v>
+      <c r="E21" s="14" t="n">
+        <v>10047</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>100</v>
+        <v>290</v>
       </c>
       <c r="H21" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21" s="14" t="n">
+        <v>10047</v>
+      </c>
       <c r="J21" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>51000305</v>
+        <v>51000304</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>121124014</v>
+        <v>121124013</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="13" t="n">
-        <v>11708</v>
+      <c r="E22" s="14" t="n">
+        <v>10026</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="G22" s="4" t="n">
-        <v>35</v>
+        <v>190</v>
       </c>
       <c r="H22" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="I22" s="14" t="n">
+        <v>10026</v>
+      </c>
       <c r="J22" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>51000306</v>
+        <v>51000304</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>121124015</v>
+        <v>121124013</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="13" t="n">
-        <v>10156</v>
+      <c r="E23" s="14" t="n">
+        <v>11709</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="G23" s="4" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H23" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="I23" s="14" t="n">
+        <v>11709</v>
+      </c>
       <c r="J23" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3617,23 +3725,26 @@
       <c r="D24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="6" t="n">
-        <v>10045</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J24" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="14" t="n">
+        <v>11708</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I24" s="14" t="n">
+        <v>11708</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3646,23 +3757,26 @@
       <c r="D25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="6" t="n">
-        <v>10048</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>240</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J25" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="14" t="n">
+        <v>10156</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="H25" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I25" s="14" t="n">
+        <v>10156</v>
+      </c>
+      <c r="J25" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3675,23 +3789,26 @@
       <c r="D26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="6" t="n">
-        <v>10028</v>
+      <c r="E26" s="7" t="n">
+        <v>10045</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>195</v>
+        <v>85</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I26" s="7" t="n">
+        <v>10045</v>
+      </c>
       <c r="J26" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3704,23 +3821,26 @@
       <c r="D27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="6" t="n">
-        <v>10031</v>
+      <c r="E27" s="7" t="n">
+        <v>10048</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I27" s="7" t="n">
+        <v>10048</v>
+      </c>
       <c r="J27" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3733,23 +3853,26 @@
       <c r="D28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="6" t="n">
-        <v>10050</v>
+      <c r="E28" s="7" t="n">
+        <v>10028</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>60</v>
+        <v>195</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I28" s="7" t="n">
+        <v>10028</v>
+      </c>
       <c r="J28" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3762,23 +3885,26 @@
       <c r="D29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="6" t="n">
-        <v>10051</v>
+      <c r="E29" s="7" t="n">
+        <v>10031</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>400</v>
+        <v>60</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I29" s="7" t="n">
+        <v>10031</v>
+      </c>
       <c r="J29" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3786,29 +3912,31 @@
         <v>22</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>121106013</v>
+        <v>121124013</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="13" t="n">
-        <v>10052</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="H30" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="E30" s="7" t="n">
+        <v>10050</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H30" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I30" s="7" t="n">
+        <v>10050</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3816,29 +3944,31 @@
         <v>22</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>121106013</v>
+        <v>121124013</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="13" t="n">
-        <v>10054</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G31" s="4" t="n">
-        <v>130</v>
-      </c>
-      <c r="H31" s="4" t="n">
-        <v>60</v>
-      </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="E31" s="7" t="n">
+        <v>10051</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I31" s="7" t="n">
+        <v>10051</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3851,24 +3981,26 @@
       <c r="D32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="13" t="n">
-        <v>10055</v>
+      <c r="E32" s="14" t="n">
+        <v>10052</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="4" t="n">
-        <v>190</v>
+        <v>100</v>
       </c>
       <c r="H32" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="14" t="n">
+        <v>10052</v>
+      </c>
       <c r="J32" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3881,24 +4013,26 @@
       <c r="D33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="13" t="n">
-        <v>10057</v>
+      <c r="E33" s="14" t="n">
+        <v>52</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G33" s="4" t="n">
-        <v>190</v>
+        <v>100</v>
       </c>
       <c r="H33" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="I33" s="14" t="n">
+        <v>52</v>
+      </c>
       <c r="J33" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3911,24 +4045,26 @@
       <c r="D34" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="13" t="n">
-        <v>10058</v>
+      <c r="E34" s="14" t="n">
+        <v>10054</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G34" s="4" t="n">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="H34" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="I34" s="14" t="n">
+        <v>10054</v>
+      </c>
       <c r="J34" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3941,24 +4077,26 @@
       <c r="D35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="13" t="n">
-        <v>10061</v>
+      <c r="E35" s="14" t="n">
+        <v>10055</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G35" s="4" t="n">
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="H35" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I35" s="4"/>
+      <c r="I35" s="14" t="n">
+        <v>10055</v>
+      </c>
       <c r="J35" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -3971,24 +4109,26 @@
       <c r="D36" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="13" t="n">
-        <v>11709</v>
+      <c r="E36" s="14" t="n">
+        <v>10057</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="G36" s="4" t="n">
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="H36" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="I36" s="14" t="n">
+        <v>10057</v>
+      </c>
       <c r="J36" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4001,54 +4141,58 @@
       <c r="D37" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="13" t="n">
-        <v>11708</v>
+      <c r="E37" s="14" t="n">
+        <v>10058</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="G37" s="4" t="n">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="H37" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="I37" s="14" t="n">
+        <v>10058</v>
+      </c>
       <c r="J37" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>51000305</v>
+        <v>51000304</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>121106014</v>
+        <v>121106013</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="13" t="n">
-        <v>10156</v>
+      <c r="E38" s="14" t="n">
+        <v>10061</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G38" s="4" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H38" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I38" s="4"/>
+      <c r="I38" s="14" t="n">
+        <v>10061</v>
+      </c>
       <c r="J38" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4061,23 +4205,26 @@
       <c r="D39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="6" t="n">
-        <v>10053</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <v>175</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J39" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="14" t="n">
+        <v>11709</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I39" s="14" t="n">
+        <v>11709</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4090,23 +4237,26 @@
       <c r="D40" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="6" t="n">
-        <v>10056</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G40" s="1" t="n">
-        <v>235</v>
-      </c>
-      <c r="H40" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J40" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="14" t="n">
+        <v>11708</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I40" s="14" t="n">
+        <v>11708</v>
+      </c>
+      <c r="J40" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4119,23 +4269,26 @@
       <c r="D41" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="6" t="n">
-        <v>10059</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G41" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="H41" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J41" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="14" t="n">
+        <v>10156</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I41" s="14" t="n">
+        <v>10156</v>
+      </c>
+      <c r="J41" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4148,23 +4301,26 @@
       <c r="D42" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="6" t="n">
-        <v>10060</v>
+      <c r="E42" s="7" t="n">
+        <v>10053</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="H42" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I42" s="7" t="n">
+        <v>10053</v>
+      </c>
       <c r="J42" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4177,23 +4333,26 @@
       <c r="D43" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="6" t="n">
-        <v>10063</v>
+      <c r="E43" s="7" t="n">
+        <v>10056</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>60</v>
+        <v>235</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I43" s="7" t="n">
+        <v>10056</v>
+      </c>
       <c r="J43" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4206,23 +4365,26 @@
       <c r="D44" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="6" t="n">
-        <v>10064</v>
+      <c r="E44" s="7" t="n">
+        <v>10059</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="G44" s="1" t="n">
-        <v>400</v>
+        <v>110</v>
       </c>
       <c r="H44" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I44" s="7" t="n">
+        <v>10059</v>
+      </c>
       <c r="J44" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4230,29 +4392,31 @@
         <v>22</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>121112023</v>
+        <v>121106013</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E45" s="13" t="n">
-        <v>10452</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G45" s="4" t="n">
-        <v>160</v>
-      </c>
-      <c r="H45" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="E45" s="7" t="n">
+        <v>10060</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G45" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I45" s="7" t="n">
+        <v>10060</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4260,29 +4424,31 @@
         <v>22</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>121112023</v>
+        <v>121106013</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E46" s="13" t="n">
-        <v>10454</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G46" s="4" t="n">
-        <v>220</v>
-      </c>
-      <c r="H46" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="E46" s="7" t="n">
+        <v>10063</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G46" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I46" s="7" t="n">
+        <v>10063</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4290,29 +4456,31 @@
         <v>22</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>121112023</v>
+        <v>121106013</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="13" t="n">
-        <v>10456</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G47" s="4" t="n">
-        <v>160</v>
-      </c>
-      <c r="H47" s="4" t="n">
-        <v>60</v>
-      </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+      <c r="E47" s="7" t="n">
+        <v>10064</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I47" s="7" t="n">
+        <v>10064</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4325,24 +4493,26 @@
       <c r="D48" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E48" s="13" t="n">
-        <v>10458</v>
+      <c r="E48" s="14" t="n">
+        <v>10452</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G48" s="4" t="n">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="H48" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I48" s="4"/>
+      <c r="I48" s="14" t="n">
+        <v>10452</v>
+      </c>
       <c r="J48" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4355,24 +4525,26 @@
       <c r="D49" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="13" t="n">
-        <v>10260</v>
+      <c r="E49" s="14" t="n">
+        <v>10454</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G49" s="4" t="n">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="H49" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I49" s="4"/>
+      <c r="I49" s="14" t="n">
+        <v>10454</v>
+      </c>
       <c r="J49" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4385,84 +4557,90 @@
       <c r="D50" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="13" t="n">
-        <v>11709</v>
+      <c r="E50" s="14" t="n">
+        <v>10456</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="G50" s="4" t="n">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="H50" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I50" s="4"/>
+      <c r="I50" s="14" t="n">
+        <v>10456</v>
+      </c>
       <c r="J50" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>51000305</v>
+        <v>51000304</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>121112024</v>
+        <v>121112023</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="13" t="n">
-        <v>11708</v>
+      <c r="E51" s="14" t="n">
+        <v>10458</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="G51" s="4" t="n">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="H51" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I51" s="4"/>
+      <c r="I51" s="14" t="n">
+        <v>10458</v>
+      </c>
       <c r="J51" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>51000306</v>
+        <v>51000304</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>121112025</v>
+        <v>121112023</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="13" t="n">
-        <v>10156</v>
+      <c r="E52" s="14" t="n">
+        <v>10260</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="G52" s="4" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H52" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I52" s="4"/>
+      <c r="I52" s="14" t="n">
+        <v>10260</v>
+      </c>
       <c r="J52" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4475,23 +4653,26 @@
       <c r="D53" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="6" t="n">
-        <v>10457</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G53" s="1" t="n">
-        <v>160</v>
-      </c>
-      <c r="H53" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J53" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="14" t="n">
+        <v>11709</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G53" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H53" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I53" s="14" t="n">
+        <v>11709</v>
+      </c>
+      <c r="J53" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4504,23 +4685,26 @@
       <c r="D54" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="6" t="n">
-        <v>10453</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G54" s="1" t="n">
-        <v>230</v>
-      </c>
-      <c r="H54" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J54" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="14" t="n">
+        <v>11708</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G54" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="H54" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I54" s="14" t="n">
+        <v>11708</v>
+      </c>
+      <c r="J54" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4533,23 +4717,26 @@
       <c r="D55" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E55" s="6" t="n">
-        <v>10455</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G55" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="H55" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J55" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="14" t="n">
+        <v>10156</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G55" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="I55" s="14" t="n">
+        <v>10156</v>
+      </c>
+      <c r="J55" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4562,23 +4749,26 @@
       <c r="D56" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E56" s="6" t="n">
-        <v>10460</v>
+      <c r="E56" s="7" t="n">
+        <v>10457</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="G56" s="1" t="n">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="H56" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I56" s="7" t="n">
+        <v>10457</v>
+      </c>
       <c r="J56" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>51000304</v>
       </c>
@@ -4591,33 +4781,132 @@
       <c r="D57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E57" s="6" t="n">
-        <v>10461</v>
+      <c r="E57" s="7" t="n">
+        <v>10453</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="G57" s="1" t="n">
-        <v>400</v>
+        <v>230</v>
       </c>
       <c r="H57" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="I57" s="7" t="n">
+        <v>10453</v>
+      </c>
       <c r="J57" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="4"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>51000304</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>121112023</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58" s="7" t="n">
+        <v>10455</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G58" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I58" s="7" t="n">
+        <v>10455</v>
+      </c>
+      <c r="J58" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>51000304</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>121112023</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E59" s="7" t="n">
+        <v>10460</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="H59" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I59" s="7" t="n">
+        <v>10460</v>
+      </c>
+      <c r="J59" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>51000304</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>121112023</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60" s="7" t="n">
+        <v>10461</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G60" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="H60" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I60" s="7" t="n">
+        <v>10461</v>
+      </c>
+      <c r="J60" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="4"/>
+    </row>
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D64" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4643,7 +4932,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="72.13"/>
@@ -4990,7 +5279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="21" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>51000298</v>
       </c>
@@ -5059,7 +5348,7 @@
       <c r="BB18" s="4"/>
       <c r="BC18" s="4"/>
     </row>
-    <row r="19" s="14" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="21" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>51000298</v>
       </c>
@@ -5846,13 +6135,13 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I53" activeCellId="0" sqref="I53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="69.39"/>
@@ -5864,39 +6153,39 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="7" t="n">
         <v>51004772</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -5908,7 +6197,7 @@
       <c r="D2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="7" t="n">
         <v>30926</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -5920,7 +6209,7 @@
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="7" t="n">
         <v>30926</v>
       </c>
       <c r="J2" s="1" t="n">
@@ -5928,7 +6217,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="7" t="n">
         <v>51004772</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -5940,7 +6229,7 @@
       <c r="D3" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="7" t="n">
         <v>30929</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -5952,15 +6241,15 @@
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="7" t="n">
         <v>30929</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -5972,27 +6261,27 @@
       <c r="D4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="24" t="n">
         <v>160</v>
       </c>
-      <c r="H4" s="17" t="n">
+      <c r="H4" s="24" t="n">
         <v>80</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="J4" s="17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="J4" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -6004,27 +6293,27 @@
       <c r="D5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="G5" s="17" t="n">
+      <c r="G5" s="24" t="n">
         <v>260</v>
       </c>
-      <c r="H5" s="17" t="n">
+      <c r="H5" s="24" t="n">
         <v>80</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="J5" s="17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="J5" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -6036,27 +6325,27 @@
       <c r="D6" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="17" t="n">
+      <c r="G6" s="24" t="n">
         <v>200</v>
       </c>
-      <c r="H6" s="17" t="n">
+      <c r="H6" s="24" t="n">
         <v>80</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="J6" s="17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+      <c r="J6" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -6068,27 +6357,27 @@
       <c r="D7" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="17" t="n">
+      <c r="G7" s="24" t="n">
         <v>170</v>
       </c>
-      <c r="H7" s="17" t="n">
+      <c r="H7" s="24" t="n">
         <v>80</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="J7" s="17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="J7" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -6100,27 +6389,27 @@
       <c r="D8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="16" t="n">
+      <c r="E8" s="23" t="n">
         <v>31709</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="17" t="n">
+      <c r="G8" s="24" t="n">
         <v>100</v>
       </c>
-      <c r="H8" s="17" t="n">
+      <c r="H8" s="24" t="n">
         <v>80</v>
       </c>
-      <c r="I8" s="16" t="n">
+      <c r="I8" s="23" t="n">
         <v>31709</v>
       </c>
-      <c r="J8" s="17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+      <c r="J8" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -6132,27 +6421,27 @@
       <c r="D9" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="16" t="n">
+      <c r="E9" s="23" t="n">
         <v>31708</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="24" t="n">
         <v>35</v>
       </c>
-      <c r="H9" s="17" t="n">
+      <c r="H9" s="24" t="n">
         <v>80</v>
       </c>
-      <c r="I9" s="16" t="n">
+      <c r="I9" s="23" t="n">
         <v>31708</v>
       </c>
-      <c r="J9" s="17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
+      <c r="J9" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -6164,27 +6453,27 @@
       <c r="D10" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E10" s="16" t="n">
+      <c r="E10" s="23" t="n">
         <v>30179</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="24" t="n">
         <v>70</v>
       </c>
-      <c r="H10" s="17" t="n">
+      <c r="H10" s="24" t="n">
         <v>80</v>
       </c>
-      <c r="I10" s="16" t="n">
+      <c r="I10" s="23" t="n">
         <v>30179</v>
       </c>
-      <c r="J10" s="17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
+      <c r="J10" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -6196,27 +6485,27 @@
       <c r="D11" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="24" t="n">
         <v>160</v>
       </c>
-      <c r="H11" s="17" t="n">
+      <c r="H11" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="J11" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="n">
+      <c r="J11" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -6228,27 +6517,27 @@
       <c r="D12" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="24" t="n">
         <v>100</v>
       </c>
-      <c r="H12" s="17" t="n">
+      <c r="H12" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="J12" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="n">
+      <c r="J12" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -6260,27 +6549,27 @@
       <c r="D13" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="17" t="n">
+      <c r="G13" s="24" t="n">
         <v>100</v>
       </c>
-      <c r="H13" s="17" t="n">
+      <c r="H13" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="J13" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
+      <c r="J13" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -6292,27 +6581,27 @@
       <c r="D14" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="G14" s="17" t="n">
+      <c r="G14" s="24" t="n">
         <v>100</v>
       </c>
-      <c r="H14" s="17" t="n">
+      <c r="H14" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="J14" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="n">
+      <c r="J14" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -6324,27 +6613,27 @@
       <c r="D15" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="17" t="n">
+      <c r="G15" s="24" t="n">
         <v>60</v>
       </c>
-      <c r="H15" s="17" t="n">
+      <c r="H15" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="J15" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="n">
+      <c r="J15" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -6356,27 +6645,27 @@
       <c r="D16" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="17" t="n">
+      <c r="G16" s="24" t="n">
         <v>400</v>
       </c>
-      <c r="H16" s="17" t="n">
+      <c r="H16" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="J16" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="n">
+      <c r="J16" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -6388,27 +6677,27 @@
       <c r="D17" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="G17" s="17" t="n">
+      <c r="G17" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="H17" s="17" t="n">
+      <c r="H17" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="n">
+      <c r="J17" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -6420,27 +6709,27 @@
       <c r="D18" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="G18" s="17" t="n">
+      <c r="G18" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="H18" s="17" t="n">
+      <c r="H18" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="J18" s="17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="n">
+      <c r="J18" s="24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -6452,7 +6741,7 @@
       <c r="D19" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E19" s="13" t="n">
+      <c r="E19" s="14" t="n">
         <v>30017</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -6464,15 +6753,15 @@
       <c r="H19" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I19" s="13" t="n">
+      <c r="I19" s="14" t="n">
         <v>30017</v>
       </c>
       <c r="J19" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="n">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -6484,7 +6773,7 @@
       <c r="D20" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E20" s="13" t="n">
+      <c r="E20" s="14" t="n">
         <v>30344</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -6496,15 +6785,15 @@
       <c r="H20" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I20" s="13" t="n">
+      <c r="I20" s="14" t="n">
         <v>30344</v>
       </c>
       <c r="J20" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="n">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -6516,7 +6805,7 @@
       <c r="D21" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E21" s="13" t="n">
+      <c r="E21" s="14" t="n">
         <v>31128</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -6528,15 +6817,15 @@
       <c r="H21" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I21" s="13" t="n">
+      <c r="I21" s="14" t="n">
         <v>31128</v>
       </c>
       <c r="J21" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="n">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -6548,7 +6837,7 @@
       <c r="D22" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="14" t="n">
         <v>31402</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -6560,15 +6849,15 @@
       <c r="H22" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I22" s="13" t="n">
+      <c r="I22" s="14" t="n">
         <v>31402</v>
       </c>
       <c r="J22" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="n">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -6580,7 +6869,7 @@
       <c r="D23" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="13" t="n">
+      <c r="E23" s="14" t="n">
         <v>31404</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -6592,15 +6881,15 @@
       <c r="H23" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I23" s="13" t="n">
+      <c r="I23" s="14" t="n">
         <v>31404</v>
       </c>
       <c r="J23" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="n">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -6612,7 +6901,7 @@
       <c r="D24" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E24" s="13" t="n">
+      <c r="E24" s="14" t="n">
         <v>31405</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -6624,79 +6913,79 @@
       <c r="H24" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I24" s="13" t="n">
+      <c r="I24" s="14" t="n">
         <v>31405</v>
       </c>
       <c r="J24" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="n">
-        <v>51000287</v>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
+        <v>51000286</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>122123044</v>
+        <v>122123043</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E25" s="16" t="n">
+      <c r="E25" s="23" t="n">
         <v>31709</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="G25" s="17" t="n">
+      <c r="G25" s="24" t="n">
         <v>100</v>
       </c>
       <c r="H25" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I25" s="13" t="n">
+      <c r="I25" s="14" t="n">
         <v>31709</v>
       </c>
       <c r="J25" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="n">
-        <v>51000288</v>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
+        <v>51000286</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>122123045</v>
+        <v>122123043</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="16" t="n">
+      <c r="E26" s="23" t="n">
         <v>31708</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="G26" s="17" t="n">
+      <c r="G26" s="24" t="n">
         <v>35</v>
       </c>
       <c r="H26" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I26" s="13" t="n">
+      <c r="I26" s="14" t="n">
         <v>31708</v>
       </c>
       <c r="J26" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="n">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -6708,27 +6997,27 @@
       <c r="D27" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E27" s="16" t="n">
+      <c r="E27" s="23" t="n">
         <v>30179</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="G27" s="17" t="n">
+      <c r="G27" s="24" t="n">
         <v>70</v>
       </c>
       <c r="H27" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I27" s="13" t="n">
+      <c r="I27" s="14" t="n">
         <v>31408</v>
       </c>
       <c r="J27" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="n">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -6740,7 +7029,7 @@
       <c r="D28" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="13" t="n">
+      <c r="E28" s="14" t="n">
         <v>31409</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -6752,15 +7041,15 @@
       <c r="H28" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I28" s="13" t="n">
+      <c r="I28" s="14" t="n">
         <v>31409</v>
       </c>
       <c r="J28" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="n">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -6772,7 +7061,7 @@
       <c r="D29" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E29" s="6" t="n">
+      <c r="E29" s="7" t="n">
         <v>30020</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -6784,15 +7073,15 @@
       <c r="H29" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I29" s="6" t="n">
+      <c r="I29" s="7" t="n">
         <v>30020</v>
       </c>
       <c r="J29" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="n">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -6804,7 +7093,7 @@
       <c r="D30" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="6" t="n">
+      <c r="E30" s="7" t="n">
         <v>31401</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -6816,15 +7105,15 @@
       <c r="H30" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I30" s="6" t="n">
+      <c r="I30" s="7" t="n">
         <v>31401</v>
       </c>
       <c r="J30" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="n">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -6836,7 +7125,7 @@
       <c r="D31" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E31" s="6" t="n">
+      <c r="E31" s="7" t="n">
         <v>31403</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -6848,15 +7137,15 @@
       <c r="H31" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I31" s="6" t="n">
+      <c r="I31" s="7" t="n">
         <v>31403</v>
       </c>
       <c r="J31" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="n">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -6868,7 +7157,7 @@
       <c r="D32" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E32" s="6" t="n">
+      <c r="E32" s="7" t="n">
         <v>31406</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -6880,15 +7169,15 @@
       <c r="H32" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I32" s="6" t="n">
+      <c r="I32" s="7" t="n">
         <v>31406</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="n">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -6900,7 +7189,7 @@
       <c r="D33" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E33" s="7" t="n">
         <v>31410</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -6912,15 +7201,15 @@
       <c r="H33" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I33" s="6" t="n">
+      <c r="I33" s="7" t="n">
         <v>31410</v>
       </c>
       <c r="J33" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="n">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -6932,7 +7221,7 @@
       <c r="D34" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E34" s="6" t="n">
+      <c r="E34" s="7" t="n">
         <v>31407</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -6944,15 +7233,15 @@
       <c r="H34" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I34" s="6" t="n">
+      <c r="I34" s="7" t="n">
         <v>31407</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="n">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -6964,7 +7253,7 @@
       <c r="D35" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E35" s="13" t="n">
+      <c r="E35" s="14" t="n">
         <v>30337</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -6976,15 +7265,15 @@
       <c r="H35" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I35" s="13" t="n">
+      <c r="I35" s="14" t="n">
         <v>30337</v>
       </c>
       <c r="J35" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="n">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -6996,7 +7285,7 @@
       <c r="D36" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E36" s="13" t="n">
+      <c r="E36" s="14" t="n">
         <v>30338</v>
       </c>
       <c r="F36" s="4" t="s">
@@ -7008,15 +7297,15 @@
       <c r="H36" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I36" s="13" t="n">
+      <c r="I36" s="14" t="n">
         <v>30338</v>
       </c>
       <c r="J36" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="n">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -7028,7 +7317,7 @@
       <c r="D37" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E37" s="13" t="n">
+      <c r="E37" s="14" t="n">
         <v>30340</v>
       </c>
       <c r="F37" s="4" t="s">
@@ -7040,15 +7329,15 @@
       <c r="H37" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I37" s="13" t="n">
+      <c r="I37" s="14" t="n">
         <v>30340</v>
       </c>
       <c r="J37" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="n">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -7060,7 +7349,7 @@
       <c r="D38" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E38" s="13" t="n">
+      <c r="E38" s="14" t="n">
         <v>30342</v>
       </c>
       <c r="F38" s="4" t="s">
@@ -7072,15 +7361,15 @@
       <c r="H38" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I38" s="13" t="n">
+      <c r="I38" s="14" t="n">
         <v>30342</v>
       </c>
       <c r="J38" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="n">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -7092,7 +7381,7 @@
       <c r="D39" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E39" s="13" t="n">
+      <c r="E39" s="14" t="n">
         <v>30344</v>
       </c>
       <c r="F39" s="4" t="s">
@@ -7104,79 +7393,79 @@
       <c r="H39" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I39" s="13" t="n">
+      <c r="I39" s="14" t="n">
         <v>30344</v>
       </c>
       <c r="J39" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="n">
-        <v>51000287</v>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="n">
+        <v>51000286</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>122123034</v>
+        <v>122123033</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="16" t="n">
+      <c r="E40" s="23" t="n">
         <v>31709</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="G40" s="17" t="n">
+      <c r="G40" s="24" t="n">
         <v>100</v>
       </c>
       <c r="H40" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I40" s="13" t="n">
+      <c r="I40" s="14" t="n">
         <v>31709</v>
       </c>
       <c r="J40" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="n">
-        <v>51000288</v>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="n">
+        <v>51000286</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>122123035</v>
+        <v>122123033</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E41" s="16" t="n">
+      <c r="E41" s="23" t="n">
         <v>31708</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="G41" s="17" t="n">
+      <c r="G41" s="24" t="n">
         <v>35</v>
       </c>
       <c r="H41" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I41" s="13" t="n">
+      <c r="I41" s="14" t="n">
         <v>31708</v>
       </c>
       <c r="J41" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="n">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -7188,27 +7477,27 @@
       <c r="D42" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E42" s="16" t="n">
+      <c r="E42" s="23" t="n">
         <v>30179</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="G42" s="17" t="n">
+      <c r="G42" s="24" t="n">
         <v>70</v>
       </c>
       <c r="H42" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="I42" s="13" t="n">
+      <c r="I42" s="14" t="n">
         <v>30346</v>
       </c>
       <c r="J42" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="n">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -7220,7 +7509,7 @@
       <c r="D43" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E43" s="6" t="n">
+      <c r="E43" s="7" t="n">
         <v>30339</v>
       </c>
       <c r="F43" s="1" t="s">
@@ -7232,15 +7521,15 @@
       <c r="H43" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I43" s="6" t="n">
+      <c r="I43" s="7" t="n">
         <v>30339</v>
       </c>
       <c r="J43" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="n">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -7252,7 +7541,7 @@
       <c r="D44" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E44" s="6" t="n">
+      <c r="E44" s="7" t="n">
         <v>30341</v>
       </c>
       <c r="F44" s="1" t="s">
@@ -7264,15 +7553,15 @@
       <c r="H44" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I44" s="6" t="n">
+      <c r="I44" s="7" t="n">
         <v>30341</v>
       </c>
       <c r="J44" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="n">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -7284,7 +7573,7 @@
       <c r="D45" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E45" s="6" t="n">
+      <c r="E45" s="7" t="n">
         <v>30343</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -7296,15 +7585,15 @@
       <c r="H45" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I45" s="6" t="n">
+      <c r="I45" s="7" t="n">
         <v>30343</v>
       </c>
       <c r="J45" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="n">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -7316,7 +7605,7 @@
       <c r="D46" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E46" s="6" t="n">
+      <c r="E46" s="7" t="n">
         <v>30020</v>
       </c>
       <c r="F46" s="1" t="s">
@@ -7328,15 +7617,15 @@
       <c r="H46" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I46" s="6" t="n">
+      <c r="I46" s="7" t="n">
         <v>30020</v>
       </c>
       <c r="J46" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="n">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -7348,7 +7637,7 @@
       <c r="D47" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E47" s="6" t="n">
+      <c r="E47" s="7" t="n">
         <v>30017</v>
       </c>
       <c r="F47" s="1" t="s">
@@ -7360,15 +7649,15 @@
       <c r="H47" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I47" s="6" t="n">
+      <c r="I47" s="7" t="n">
         <v>30017</v>
       </c>
       <c r="J47" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="n">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -7380,7 +7669,7 @@
       <c r="D48" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E48" s="6" t="n">
+      <c r="E48" s="7" t="n">
         <v>30347</v>
       </c>
       <c r="F48" s="1" t="s">
@@ -7392,15 +7681,15 @@
       <c r="H48" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I48" s="6" t="n">
+      <c r="I48" s="7" t="n">
         <v>30347</v>
       </c>
       <c r="J48" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="n">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -7412,7 +7701,7 @@
       <c r="D49" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E49" s="6" t="n">
+      <c r="E49" s="7" t="n">
         <v>30348</v>
       </c>
       <c r="F49" s="1" t="s">
@@ -7424,15 +7713,15 @@
       <c r="H49" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I49" s="6" t="n">
+      <c r="I49" s="7" t="n">
         <v>30348</v>
       </c>
       <c r="J49" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="n">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7" t="n">
         <v>51000286</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -7444,7 +7733,7 @@
       <c r="D50" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E50" s="6" t="n">
+      <c r="E50" s="7" t="n">
         <v>30345</v>
       </c>
       <c r="F50" s="1" t="s">
@@ -7456,7 +7745,7 @@
       <c r="H50" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="I50" s="6" t="n">
+      <c r="I50" s="7" t="n">
         <v>30345</v>
       </c>
       <c r="J50" s="1" t="n">
@@ -7479,10 +7768,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7532,32 +7821,33 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>51000304</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>125112014</v>
-      </c>
-      <c r="D3" s="4" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>51004772</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="25" t="n">
+        <v>124120013</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>187</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>51000304</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="n">
-        <v>125124014</v>
+      <c r="C4" s="26" t="n">
+        <v>124112024</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>188</v>
@@ -7565,6 +7855,43 @@
       <c r="E4" s="1" t="n">
         <v>30</v>
       </c>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>51000304</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="26" t="n">
+        <v>125112014</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>51000304</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>125124014</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7624,7 +7951,7 @@
         <v>124120013</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>60</v>

</xml_diff>